<commit_message>
Use function to round and preserv sum
</commit_message>
<xml_diff>
--- a/inst/extdata/mechanisms.xlsx
+++ b/inst/extdata/mechanisms.xlsx
@@ -470,7 +470,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5">
@@ -504,7 +504,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7">
@@ -555,7 +555,7 @@
         <v>35</v>
       </c>
       <c r="E9" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10">
@@ -589,7 +589,7 @@
         <v>35</v>
       </c>
       <c r="E11" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="12">
@@ -640,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="15">
@@ -674,7 +674,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         <v>55</v>
       </c>
       <c r="E18" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19">
@@ -759,7 +759,7 @@
         <v>55</v>
       </c>
       <c r="E21" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
@@ -912,7 +912,7 @@
         <v>80</v>
       </c>
       <c r="E30" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="31">
@@ -929,7 +929,7 @@
         <v>80</v>
       </c>
       <c r="E31" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32">
@@ -963,7 +963,7 @@
         <v>55</v>
       </c>
       <c r="E33" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34">
@@ -980,7 +980,7 @@
         <v>55</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1048,7 +1048,7 @@
         <v>40</v>
       </c>
       <c r="E38" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="39">
@@ -1099,7 +1099,7 @@
         <v>40</v>
       </c>
       <c r="E41" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="42">
@@ -1422,7 +1422,7 @@
         <v>65</v>
       </c>
       <c r="E60" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="61">
@@ -1439,7 +1439,7 @@
         <v>65</v>
       </c>
       <c r="E61" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="62">
@@ -1490,7 +1490,7 @@
         <v>55</v>
       </c>
       <c r="E64" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="65">
@@ -1524,7 +1524,7 @@
         <v>55</v>
       </c>
       <c r="E66" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="67">
@@ -1592,7 +1592,7 @@
         <v>35</v>
       </c>
       <c r="E70" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="71">
@@ -1609,7 +1609,7 @@
         <v>35</v>
       </c>
       <c r="E71" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="72">
@@ -1813,7 +1813,7 @@
         <v>40</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="84">
@@ -1830,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="E84" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="85">
@@ -1983,7 +1983,7 @@
         <v>55</v>
       </c>
       <c r="E93" t="n">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="94">
@@ -2034,7 +2034,7 @@
         <v>55</v>
       </c>
       <c r="E96" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97">
@@ -2238,7 +2238,7 @@
         <v>90</v>
       </c>
       <c r="E108" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="109">
@@ -2289,7 +2289,7 @@
         <v>90</v>
       </c>
       <c r="E111" t="n">
-        <v>0.00999999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="112">
@@ -2442,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="E120" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="121">
@@ -2459,7 +2459,7 @@
         <v>35</v>
       </c>
       <c r="E121" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -2609,7 +2609,7 @@
         <v>20</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
@@ -2643,7 +2643,7 @@
         <v>20</v>
       </c>
       <c r="E10" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="11">
@@ -2660,7 +2660,7 @@
         <v>20</v>
       </c>
       <c r="E11" t="n">
-        <v>0.31</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="12">
@@ -2796,7 +2796,7 @@
         <v>70</v>
       </c>
       <c r="E19" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="20">
@@ -2830,7 +2830,7 @@
         <v>70</v>
       </c>
       <c r="E21" t="n">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="22">
@@ -2881,7 +2881,7 @@
         <v>75</v>
       </c>
       <c r="E24" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="25">
@@ -2915,7 +2915,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="27">
@@ -2966,7 +2966,7 @@
         <v>95</v>
       </c>
       <c r="E29" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="30">
@@ -3000,7 +3000,7 @@
         <v>95</v>
       </c>
       <c r="E31" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="32">
@@ -3034,7 +3034,7 @@
         <v>35</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34">
@@ -3085,7 +3085,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="37">
@@ -3153,7 +3153,7 @@
         <v>5</v>
       </c>
       <c r="E40" t="n">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="41">
@@ -3170,7 +3170,7 @@
         <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.00000000000000000867361737988404</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42">
@@ -3204,7 +3204,7 @@
         <v>100</v>
       </c>
       <c r="E43" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="44">
@@ -3238,7 +3238,7 @@
         <v>100</v>
       </c>
       <c r="E45" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="46">
@@ -3289,7 +3289,7 @@
         <v>100</v>
       </c>
       <c r="E48" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49">
@@ -3340,7 +3340,7 @@
         <v>100</v>
       </c>
       <c r="E51" t="n">
-        <v>0.69</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="52">
@@ -3578,7 +3578,7 @@
         <v>80</v>
       </c>
       <c r="E65" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="66">
@@ -3595,7 +3595,7 @@
         <v>80</v>
       </c>
       <c r="E66" t="n">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="67">
@@ -3663,7 +3663,7 @@
         <v>35</v>
       </c>
       <c r="E70" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="71">
@@ -3680,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="72">
@@ -3731,7 +3731,7 @@
         <v>15</v>
       </c>
       <c r="E74" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="75">
@@ -3748,7 +3748,7 @@
         <v>15</v>
       </c>
       <c r="E75" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="76">
@@ -3884,7 +3884,7 @@
         <v>15</v>
       </c>
       <c r="E83" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="84">
@@ -3901,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="E84" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="85">
@@ -3969,7 +3969,7 @@
         <v>5</v>
       </c>
       <c r="E88" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="89">
@@ -4003,7 +4003,7 @@
         <v>5</v>
       </c>
       <c r="E90" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="91">
@@ -4054,7 +4054,7 @@
         <v>55</v>
       </c>
       <c r="E93" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="94">
@@ -4105,7 +4105,7 @@
         <v>55</v>
       </c>
       <c r="E96" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="97">
@@ -4374,7 +4374,7 @@
         <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="11">
@@ -4391,7 +4391,7 @@
         <v>50</v>
       </c>
       <c r="E11" t="n">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="12">
@@ -4714,7 +4714,7 @@
         <v>55</v>
       </c>
       <c r="E30" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31">
@@ -4731,7 +4731,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32">
@@ -4765,7 +4765,7 @@
         <v>60</v>
       </c>
       <c r="E33" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="34">
@@ -4799,7 +4799,7 @@
         <v>60</v>
       </c>
       <c r="E35" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="36">
@@ -4884,7 +4884,7 @@
         <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="41">
@@ -4901,7 +4901,7 @@
         <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="42">
@@ -4969,7 +4969,7 @@
         <v>75</v>
       </c>
       <c r="E45" t="n">
-        <v>0.56</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="46">
@@ -4986,7 +4986,7 @@
         <v>75</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="47">
@@ -5105,7 +5105,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="54">
@@ -5156,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0599999999999999</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="57">
@@ -5190,7 +5190,7 @@
         <v>70</v>
       </c>
       <c r="E58" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59">
@@ -5241,7 +5241,7 @@
         <v>70</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="62">
@@ -5292,7 +5292,7 @@
         <v>95</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65">
@@ -5326,7 +5326,7 @@
         <v>95</v>
       </c>
       <c r="E66" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="67">
@@ -5479,7 +5479,7 @@
         <v>55</v>
       </c>
       <c r="E75" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="76">
@@ -5496,7 +5496,7 @@
         <v>55</v>
       </c>
       <c r="E76" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="77">
@@ -5564,7 +5564,7 @@
         <v>75</v>
       </c>
       <c r="E80" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="81">
@@ -5581,7 +5581,7 @@
         <v>75</v>
       </c>
       <c r="E81" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="82">
@@ -5717,7 +5717,7 @@
         <v>35</v>
       </c>
       <c r="E89" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="90">
@@ -5734,7 +5734,7 @@
         <v>35</v>
       </c>
       <c r="E90" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="91">

</xml_diff>

<commit_message>
Create function to plot sampled categorical data (#74)
</commit_message>
<xml_diff>
--- a/inst/extdata/mechanisms.xlsx
+++ b/inst/extdata/mechanisms.xlsx
@@ -470,7 +470,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5">
@@ -504,7 +504,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7">
@@ -555,7 +555,7 @@
         <v>35</v>
       </c>
       <c r="E9" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="10">
@@ -589,7 +589,7 @@
         <v>35</v>
       </c>
       <c r="E11" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="12">
@@ -640,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="15">
@@ -674,7 +674,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         <v>55</v>
       </c>
       <c r="E18" t="n">
-        <v>0.61</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19">
@@ -759,7 +759,7 @@
         <v>55</v>
       </c>
       <c r="E21" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
@@ -912,7 +912,7 @@
         <v>80</v>
       </c>
       <c r="E30" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="31">
@@ -929,7 +929,7 @@
         <v>80</v>
       </c>
       <c r="E31" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32">
@@ -963,7 +963,7 @@
         <v>55</v>
       </c>
       <c r="E33" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34">
@@ -980,7 +980,7 @@
         <v>55</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1048,7 +1048,7 @@
         <v>40</v>
       </c>
       <c r="E38" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="39">
@@ -1099,7 +1099,7 @@
         <v>40</v>
       </c>
       <c r="E41" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="42">
@@ -1422,7 +1422,7 @@
         <v>65</v>
       </c>
       <c r="E60" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="61">
@@ -1439,7 +1439,7 @@
         <v>65</v>
       </c>
       <c r="E61" t="n">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="62">
@@ -1490,7 +1490,7 @@
         <v>55</v>
       </c>
       <c r="E64" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="65">
@@ -1524,7 +1524,7 @@
         <v>55</v>
       </c>
       <c r="E66" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="67">
@@ -1592,7 +1592,7 @@
         <v>35</v>
       </c>
       <c r="E70" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="71">
@@ -1609,7 +1609,7 @@
         <v>35</v>
       </c>
       <c r="E71" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="72">
@@ -1813,7 +1813,7 @@
         <v>40</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="84">
@@ -1830,7 +1830,7 @@
         <v>40</v>
       </c>
       <c r="E84" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="85">
@@ -1983,7 +1983,7 @@
         <v>55</v>
       </c>
       <c r="E93" t="n">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="94">
@@ -2034,7 +2034,7 @@
         <v>55</v>
       </c>
       <c r="E96" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="97">
@@ -2238,7 +2238,7 @@
         <v>90</v>
       </c>
       <c r="E108" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="109">
@@ -2289,7 +2289,7 @@
         <v>90</v>
       </c>
       <c r="E111" t="n">
-        <v>0.00999999999999999</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="112">
@@ -2442,7 +2442,7 @@
         <v>35</v>
       </c>
       <c r="E120" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="121">
@@ -2459,7 +2459,7 @@
         <v>35</v>
       </c>
       <c r="E121" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -2609,7 +2609,7 @@
         <v>20</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
@@ -2643,7 +2643,7 @@
         <v>20</v>
       </c>
       <c r="E10" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="11">
@@ -2660,7 +2660,7 @@
         <v>20</v>
       </c>
       <c r="E11" t="n">
-        <v>0.31</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="12">
@@ -2796,7 +2796,7 @@
         <v>70</v>
       </c>
       <c r="E19" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="20">
@@ -2830,7 +2830,7 @@
         <v>70</v>
       </c>
       <c r="E21" t="n">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="22">
@@ -2881,7 +2881,7 @@
         <v>75</v>
       </c>
       <c r="E24" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="25">
@@ -2915,7 +2915,7 @@
         <v>75</v>
       </c>
       <c r="E26" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="27">
@@ -2966,7 +2966,7 @@
         <v>95</v>
       </c>
       <c r="E29" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="30">
@@ -3000,7 +3000,7 @@
         <v>95</v>
       </c>
       <c r="E31" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="32">
@@ -3034,7 +3034,7 @@
         <v>35</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34">
@@ -3085,7 +3085,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="n">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="37">
@@ -3153,7 +3153,7 @@
         <v>5</v>
       </c>
       <c r="E40" t="n">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="41">
@@ -3170,7 +3170,7 @@
         <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.00000000000000000867361737988404</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42">
@@ -3204,7 +3204,7 @@
         <v>100</v>
       </c>
       <c r="E43" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="44">
@@ -3238,7 +3238,7 @@
         <v>100</v>
       </c>
       <c r="E45" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="46">
@@ -3289,7 +3289,7 @@
         <v>100</v>
       </c>
       <c r="E48" t="n">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49">
@@ -3340,7 +3340,7 @@
         <v>100</v>
       </c>
       <c r="E51" t="n">
-        <v>0.69</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="52">
@@ -3578,7 +3578,7 @@
         <v>80</v>
       </c>
       <c r="E65" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="66">
@@ -3595,7 +3595,7 @@
         <v>80</v>
       </c>
       <c r="E66" t="n">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="67">
@@ -3663,7 +3663,7 @@
         <v>35</v>
       </c>
       <c r="E70" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="71">
@@ -3680,7 +3680,7 @@
         <v>35</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="72">
@@ -3731,7 +3731,7 @@
         <v>15</v>
       </c>
       <c r="E74" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="75">
@@ -3748,7 +3748,7 @@
         <v>15</v>
       </c>
       <c r="E75" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="76">
@@ -3884,7 +3884,7 @@
         <v>15</v>
       </c>
       <c r="E83" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="84">
@@ -3901,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="E84" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="85">
@@ -3969,7 +3969,7 @@
         <v>5</v>
       </c>
       <c r="E88" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="89">
@@ -4003,7 +4003,7 @@
         <v>5</v>
       </c>
       <c r="E90" t="n">
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="91">
@@ -4054,7 +4054,7 @@
         <v>55</v>
       </c>
       <c r="E93" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="94">
@@ -4105,7 +4105,7 @@
         <v>55</v>
       </c>
       <c r="E96" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="97">
@@ -4374,7 +4374,7 @@
         <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="11">
@@ -4391,7 +4391,7 @@
         <v>50</v>
       </c>
       <c r="E11" t="n">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="12">
@@ -4714,7 +4714,7 @@
         <v>55</v>
       </c>
       <c r="E30" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="31">
@@ -4731,7 +4731,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="n">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32">
@@ -4765,7 +4765,7 @@
         <v>60</v>
       </c>
       <c r="E33" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="34">
@@ -4799,7 +4799,7 @@
         <v>60</v>
       </c>
       <c r="E35" t="n">
-        <v>0.23</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="36">
@@ -4884,7 +4884,7 @@
         <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="41">
@@ -4901,7 +4901,7 @@
         <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="42">
@@ -4969,7 +4969,7 @@
         <v>75</v>
       </c>
       <c r="E45" t="n">
-        <v>0.56</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="46">
@@ -4986,7 +4986,7 @@
         <v>75</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="47">
@@ -5105,7 +5105,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="54">
@@ -5156,7 +5156,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0599999999999999</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="57">
@@ -5190,7 +5190,7 @@
         <v>70</v>
       </c>
       <c r="E58" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59">
@@ -5241,7 +5241,7 @@
         <v>70</v>
       </c>
       <c r="E61" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="62">
@@ -5292,7 +5292,7 @@
         <v>95</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65">
@@ -5326,7 +5326,7 @@
         <v>95</v>
       </c>
       <c r="E66" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="67">
@@ -5479,7 +5479,7 @@
         <v>55</v>
       </c>
       <c r="E75" t="n">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="76">
@@ -5496,7 +5496,7 @@
         <v>55</v>
       </c>
       <c r="E76" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="77">
@@ -5564,7 +5564,7 @@
         <v>75</v>
       </c>
       <c r="E80" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="81">
@@ -5581,7 +5581,7 @@
         <v>75</v>
       </c>
       <c r="E81" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="82">
@@ -5717,7 +5717,7 @@
         <v>35</v>
       </c>
       <c r="E89" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="90">
@@ -5734,7 +5734,7 @@
         <v>35</v>
       </c>
       <c r="E90" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="91">

</xml_diff>